<commit_message>
removed uploadefile step from sharepoint assets deployment. It will be part of azure deployment.
</commit_message>
<xml_diff>
--- a/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
+++ b/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mc\tree\master\cloud\src\deployments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mc\tree\master\cloud\src\deployments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="62316" yWindow="0" windowWidth="24276" windowHeight="12276" tabRatio="822" activeTab="1"/>
+    <workbookView xWindow="62310" yWindow="0" windowWidth="24270" windowHeight="12270" tabRatio="822" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="11" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="120">
   <si>
     <t>Group_Name</t>
   </si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t xml:space="preserve">Kindly refer to Deployment Document present in docs folder to learn how to use this file </t>
+  </si>
+  <si>
+    <t>IsDeployedonAzure</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -635,6 +638,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -953,43 +959,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="32.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75" customWidth="1"/>
-    <col min="4" max="4" width="82.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="10"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" s="10"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
     </row>
   </sheetData>
@@ -1000,20 +1006,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="88.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="193.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="193.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>48</v>
       </c>
@@ -1024,7 +1030,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1036,7 +1042,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
@@ -1047,7 +1053,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1058,7 +1064,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1069,7 +1075,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1080,7 +1086,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1089,6 +1095,14 @@
       </c>
       <c r="C7" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="19" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1110,15 +1124,15 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="88.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="88.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1146,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1146,7 +1160,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1174,20 +1188,20 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="34.375" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="5" width="15.375" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.5546875" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" customWidth="1"/>
-    <col min="9" max="9" width="26.88671875" customWidth="1"/>
+    <col min="7" max="7" width="40.5" customWidth="1"/>
+    <col min="8" max="8" width="23.375" customWidth="1"/>
+    <col min="9" max="9" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -1216,7 +1230,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1245,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1274,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1303,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1332,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1361,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1390,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1419,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1448,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1477,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1506,7 +1520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -1535,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -1576,16 +1590,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.5546875" customWidth="1"/>
-    <col min="5" max="5" width="67.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.5" customWidth="1"/>
+    <col min="5" max="5" width="67.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -1602,7 +1616,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>114</v>
       </c>
@@ -1619,126 +1633,126 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -1759,29 +1773,29 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="131.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" customWidth="1"/>
-    <col min="18" max="18" width="26.33203125" customWidth="1"/>
+    <col min="6" max="6" width="39.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="131.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.375" customWidth="1"/>
+    <col min="17" max="17" width="18.5" customWidth="1"/>
+    <col min="18" max="18" width="26.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>26</v>
       </c>
@@ -1828,7 +1842,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>116</v>
       </c>
@@ -1875,7 +1889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>116</v>
       </c>
@@ -1922,7 +1936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>116</v>
       </c>
@@ -1969,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>116</v>
       </c>
@@ -2016,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>116</v>
       </c>
@@ -2063,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>116</v>
       </c>
@@ -2110,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>116</v>
       </c>
@@ -2157,7 +2171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>116</v>
       </c>
@@ -2204,7 +2218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>116</v>
       </c>
@@ -2251,7 +2265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>116</v>
       </c>
@@ -2298,7 +2312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>116</v>
       </c>
@@ -2345,7 +2359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>116</v>
       </c>
@@ -2392,7 +2406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>116</v>
       </c>
@@ -2439,7 +2453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>116</v>
       </c>
@@ -2486,7 +2500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
1. Removed IsDeployOnAzure. 2. Removed exe, dll that will be genarated as part of compilation
</commit_message>
<xml_diff>
--- a/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
+++ b/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="117">
   <si>
     <t>Group_Name</t>
   </si>
@@ -161,12 +161,6 @@
   </si>
   <si>
     <t>Provision Matter Users</t>
-  </si>
-  <si>
-    <t>IsLoggingOnAzure</t>
-  </si>
-  <si>
-    <t>Flag to differentiate where the logging is carried out</t>
   </si>
   <si>
     <t>Matter Center Users</t>
@@ -494,9 +488,6 @@
   </si>
   <si>
     <t xml:space="preserve">Kindly refer to Deployment Document present in docs folder to learn how to use this file </t>
-  </si>
-  <si>
-    <t>IsDeployedonAzure</t>
   </si>
 </sst>
 </file>
@@ -596,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -613,9 +604,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -638,9 +626,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,8 +952,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>117</v>
+      <c r="A1" s="17" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -976,27 +961,27 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
-      <c r="D4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="10"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="10"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="10"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="10"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="10"/>
+      <c r="C15" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1006,10 +991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,20 +1006,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>109</v>
+        <v>46</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>107</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="11" t="str">
+      <c r="B2" s="10" t="str">
         <f>CONCATENATE(B1, "/sites/contentTypeHub")</f>
         <v>https://&lt;TENANTNAME&gt;.sharepoint.com/sites/contentTypeHub</v>
       </c>
@@ -1046,8 +1031,8 @@
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>110</v>
+      <c r="B3" s="10" t="s">
+        <v>108</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>38</v>
@@ -1057,8 +1042,8 @@
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>111</v>
+      <c r="B4" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
@@ -1066,48 +1051,29 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="8" t="b">
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
         <v>55</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="19" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>"Email Only, Document Only, Both"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1148,16 +1114,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>112</v>
+        <v>52</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1168,10 +1134,10 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>112</v>
+        <v>52</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1203,31 +1169,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1241,13 +1207,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>6</v>
@@ -1270,13 +1236,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>7</v>
@@ -1299,13 +1265,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>8</v>
@@ -1328,13 +1294,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>9</v>
@@ -1357,13 +1323,13 @@
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>11</v>
@@ -1386,13 +1352,13 @@
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -1415,13 +1381,13 @@
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>13</v>
@@ -1444,13 +1410,13 @@
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>14</v>
@@ -1473,13 +1439,13 @@
         <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>16</v>
@@ -1502,13 +1468,13 @@
         <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>17</v>
@@ -1531,13 +1497,13 @@
         <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>19</v>
@@ -1560,13 +1526,13 @@
         <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>20</v>
@@ -1610,154 +1576,154 @@
         <v>36</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="16">
+      <c r="A2" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="15">
         <v>100001</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>112</v>
+      <c r="C2" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1783,7 +1749,7 @@
     <col min="6" max="6" width="39.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="131.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.875" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.625" bestFit="1" customWidth="1"/>
@@ -1796,138 +1762,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="F2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="13">
+        <v>43904</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="12" t="s">
+      <c r="C3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="13">
+        <v>44270</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K3" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="14">
-        <v>43904</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="L2" s="11" t="s">
+      <c r="L3" t="s">
         <v>105</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="N2" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O2" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I3" s="14">
-        <v>44270</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K3" t="s">
-        <v>106</v>
-      </c>
-      <c r="L3" t="s">
-        <v>107</v>
-      </c>
       <c r="M3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N3" t="b">
         <v>0</v>
@@ -1937,44 +1903,44 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>116</v>
+      <c r="A4" s="14" t="s">
+        <v>114</v>
       </c>
       <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="11" t="s">
+      <c r="E4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" s="13">
+        <v>44636</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="14">
-        <v>44636</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>106</v>
-      </c>
       <c r="L4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N4" t="b">
         <v>1</v>
@@ -1984,566 +1950,566 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" s="13">
+        <v>45002</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="N5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="C6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="E6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="13">
+        <v>45368</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="I5" s="14">
-        <v>45002</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="L5" s="11" t="s">
+      <c r="L6" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="N6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="13">
+        <v>45734</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="N5" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" s="11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="11" t="s">
+      <c r="L7" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="N7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H8" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" s="13">
+        <v>46100</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="N8" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="13">
+        <v>46466</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K9" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="I6" s="14">
-        <v>45368</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K6" s="11" t="s">
+      <c r="L9" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="N9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" s="13">
+        <v>46832</v>
+      </c>
+      <c r="J10" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="L6" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="M6" s="11" t="s">
+      <c r="K10" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="N6" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O6" s="11" t="b">
+      <c r="L10" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="N10" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="11" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H11" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I11" s="13">
+        <v>47198</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="N11" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" s="13">
+        <v>47564</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="I7" s="14">
-        <v>45734</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K7" s="11" t="s">
+      <c r="L12" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="N12" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="13">
+        <v>47930</v>
+      </c>
+      <c r="J13" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="K13" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="M7" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="N7" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" s="11" t="b">
+      <c r="L13" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="N13" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" s="10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="11" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H14" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="13">
+        <v>48296</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="N14" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="13">
+        <v>48662</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K15" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="14">
-        <v>46100</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="L8" s="11" t="s">
+      <c r="L15" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="M15" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="N15" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16" s="13">
+        <v>49028</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="N8" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I9" s="14">
-        <v>46466</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="N9" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O9" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I10" s="14">
-        <v>46832</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="N10" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" s="14">
-        <v>47198</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="L11" s="11" t="s">
+      <c r="L16" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="M16" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="M11" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="N11" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O11" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I12" s="14">
-        <v>47564</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="M12" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="N12" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O12" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I13" s="14">
-        <v>47930</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="M13" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="N13" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O13" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I14" s="14">
-        <v>48296</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="M14" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="N14" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O14" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I15" s="14">
-        <v>48662</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="M15" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="N15" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O15" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I16" s="14">
-        <v>49028</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="N16" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O16" s="11" t="b">
+      <c r="N16" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="10" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update CatalogSiteURL in MCDeploymentConfig.xlsx  to pint to sites instaed of teams
</commit_message>
<xml_diff>
--- a/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
+++ b/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mc\tree\master\cloud\src\deployments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\mattercenter2\tree\master\cloud\src\deployments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -402,45 +402,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.sharepoint.com/teams/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;CATALOGNAME&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>https://</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;TENANTNAME&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>-admin.sharepoint.com</t>
     </r>
   </si>
@@ -488,6 +449,45 @@
   </si>
   <si>
     <t xml:space="preserve">Kindly refer to Deployment Document present in docs folder to learn how to use this file </t>
+  </si>
+  <si>
+    <r>
+      <t>https://</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;TENANTNAME&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.sharepoint.com/sites/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;CATALOGNAME&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -946,14 +946,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75" customWidth="1"/>
-    <col min="4" max="4" width="82.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -994,14 +994,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="88.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="193.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="193.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1032,7 +1032,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>38</v>
@@ -1043,7 +1043,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
@@ -1092,10 +1092,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" customWidth="1"/>
-    <col min="4" max="4" width="88.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="88.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1123,7 +1123,7 @@
         <v>52</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>52</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1156,15 +1156,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="34.375" customWidth="1"/>
-    <col min="4" max="4" width="15.125" customWidth="1"/>
-    <col min="5" max="5" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.5" customWidth="1"/>
-    <col min="8" max="8" width="23.375" customWidth="1"/>
-    <col min="9" max="9" width="26.875" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1207,13 +1207,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>6</v>
@@ -1236,13 +1236,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>7</v>
@@ -1265,13 +1265,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>8</v>
@@ -1294,13 +1294,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>9</v>
@@ -1323,13 +1323,13 @@
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>11</v>
@@ -1352,13 +1352,13 @@
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -1381,13 +1381,13 @@
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>13</v>
@@ -1410,13 +1410,13 @@
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>14</v>
@@ -1439,13 +1439,13 @@
         <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>16</v>
@@ -1468,13 +1468,13 @@
         <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>17</v>
@@ -1497,13 +1497,13 @@
         <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>19</v>
@@ -1526,13 +1526,13 @@
         <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>20</v>
@@ -1558,11 +1558,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.5" customWidth="1"/>
-    <col min="5" max="5" width="67.375" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.42578125" customWidth="1"/>
+    <col min="5" max="5" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1584,19 +1584,19 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="15">
         <v>100001</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1741,24 +1741,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="131.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.375" customWidth="1"/>
-    <col min="17" max="17" width="18.5" customWidth="1"/>
-    <col min="18" max="18" width="26.375" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="131.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.42578125" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" customWidth="1"/>
+    <col min="18" max="18" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1810,7 +1810,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>72</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
         <v>73</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
         <v>74</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>77</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>79</v>
@@ -2045,7 +2045,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>81</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>83</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>85</v>
@@ -2186,7 +2186,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>87</v>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>89</v>
@@ -2280,7 +2280,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>91</v>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>93</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>95</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>97</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Fix for  issue #598  deployment error on key vault, no search source id #598  (#600)
* Changes for CloudConnection string to ensure lower case in the keyVault
Added code to build the RedisConenctionstring to be stored in the KeyVault

* Changes for Redis Ccahe Connection strring  in Key Vault

* Parameter

* Removed extra empty spaces

* Change SearchResultSourceID to be read from Tenat live instead of catalog level

* Change SearchResultSourceID to be read from Tenat live instead of catalog level

* Revert "Change SearchResultSourceID to be read from Tenat live instead of catalog level"

This reverts commit c8057a67df31b97bc687e559c6d0443b7b25b218.

* Recommit

* Ignore log files

* Remove extra file and remove deployment path from .gitignore

* Update CatalogSiteURL in MCDeploymentConfig.xlsx  to pint to sites instaed of teams
</commit_message>
<xml_diff>
--- a/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
+++ b/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mc\tree\master\cloud\src\deployments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\mattercenter2\tree\master\cloud\src\deployments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -402,45 +402,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.sharepoint.com/teams/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;CATALOGNAME&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>https://</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;TENANTNAME&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>-admin.sharepoint.com</t>
     </r>
   </si>
@@ -488,6 +449,45 @@
   </si>
   <si>
     <t xml:space="preserve">Kindly refer to Deployment Document present in docs folder to learn how to use this file </t>
+  </si>
+  <si>
+    <r>
+      <t>https://</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;TENANTNAME&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.sharepoint.com/sites/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;CATALOGNAME&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -946,14 +946,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75" customWidth="1"/>
-    <col min="4" max="4" width="82.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -994,14 +994,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="88.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="193.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="193.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1032,7 +1032,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>38</v>
@@ -1043,7 +1043,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
@@ -1092,10 +1092,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" customWidth="1"/>
-    <col min="4" max="4" width="88.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="88.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1123,7 +1123,7 @@
         <v>52</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>52</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1156,15 +1156,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="34.375" customWidth="1"/>
-    <col min="4" max="4" width="15.125" customWidth="1"/>
-    <col min="5" max="5" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.5" customWidth="1"/>
-    <col min="8" max="8" width="23.375" customWidth="1"/>
-    <col min="9" max="9" width="26.875" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1207,13 +1207,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>6</v>
@@ -1236,13 +1236,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>7</v>
@@ -1265,13 +1265,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>8</v>
@@ -1294,13 +1294,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>9</v>
@@ -1323,13 +1323,13 @@
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>11</v>
@@ -1352,13 +1352,13 @@
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -1381,13 +1381,13 @@
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>13</v>
@@ -1410,13 +1410,13 @@
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>14</v>
@@ -1439,13 +1439,13 @@
         <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>16</v>
@@ -1468,13 +1468,13 @@
         <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>17</v>
@@ -1497,13 +1497,13 @@
         <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>19</v>
@@ -1526,13 +1526,13 @@
         <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>20</v>
@@ -1558,11 +1558,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.5" customWidth="1"/>
-    <col min="5" max="5" width="67.375" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.42578125" customWidth="1"/>
+    <col min="5" max="5" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1584,19 +1584,19 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="15">
         <v>100001</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1741,24 +1741,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="131.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.375" customWidth="1"/>
-    <col min="17" max="17" width="18.5" customWidth="1"/>
-    <col min="18" max="18" width="26.375" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="131.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.42578125" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" customWidth="1"/>
+    <col min="18" max="18" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1810,7 +1810,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>72</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
         <v>73</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
         <v>74</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>77</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>79</v>
@@ -2045,7 +2045,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>81</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>83</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>85</v>
@@ -2186,7 +2186,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>87</v>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>89</v>
@@ -2280,7 +2280,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>91</v>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>93</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>95</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>97</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
New Powershell script for adding additional matter properties when provisioning matter
</commit_message>
<xml_diff>
--- a/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
+++ b/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\mattercenter2\tree\master\cloud\src\deployments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\mc\tree\master\cloud\src\deployments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="62310" yWindow="0" windowWidth="24270" windowHeight="12270" tabRatio="822" activeTab="1"/>
+    <workbookView xWindow="62310" yWindow="0" windowWidth="24270" windowHeight="12270" tabRatio="822" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="11" r:id="rId1"/>
@@ -17,7 +17,8 @@
     <sheet name="Create_Group" sheetId="3" r:id="rId3"/>
     <sheet name="TermStore_Config" sheetId="4" r:id="rId4"/>
     <sheet name="Client_Config" sheetId="8" r:id="rId5"/>
-    <sheet name="Sample_Data" sheetId="9" r:id="rId6"/>
+    <sheet name="MatterAdditionalColumns" sheetId="12" r:id="rId6"/>
+    <sheet name="Sample_Data" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027" forceFullCalc="1"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="140">
   <si>
     <t>Group_Name</t>
   </si>
@@ -489,12 +490,81 @@
       <t>&lt;CATALOGNAME&gt;</t>
     </r>
   </si>
+  <si>
+    <t>SiteColumnName</t>
+  </si>
+  <si>
+    <t>ColumnType</t>
+  </si>
+  <si>
+    <t>SubColumnType</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>MatterAdditionalComments</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>_MatterCenter</t>
+  </si>
+  <si>
+    <t>IsClientCritical</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>MatterClosureDate</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>IsMatterDuplicate</t>
+  </si>
+  <si>
+    <t>MatterUploadOptions</t>
+  </si>
+  <si>
+    <t>Choice</t>
+  </si>
+  <si>
+    <t>RadioButtons</t>
+  </si>
+  <si>
+    <t>Emails, Attachments,Desktop</t>
+  </si>
+  <si>
+    <t>MatterRelatedTo</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>Patents,Copyrights,Infringements</t>
+  </si>
+  <si>
+    <t>MatterFiledAgainst</t>
+  </si>
+  <si>
+    <t>MultiChoice</t>
+  </si>
+  <si>
+    <t>Contoso,Fabrikam</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,8 +615,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -559,8 +647,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7D31"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -583,11 +677,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -626,6 +744,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -993,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1732,6 +1860,146 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O16"/>
   <sheetViews>

</xml_diff>

<commit_message>
New Powershell script for adding additional matter properties when provisioning matter (#724)
* New Powershell script for adding additional matter properties when provisioning matter

* Updated the powershell script to read content type from user
</commit_message>
<xml_diff>
--- a/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
+++ b/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\mattercenter2\tree\master\cloud\src\deployments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\mc\tree\master\cloud\src\deployments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="62310" yWindow="0" windowWidth="24270" windowHeight="12270" tabRatio="822" activeTab="1"/>
+    <workbookView xWindow="62310" yWindow="0" windowWidth="24270" windowHeight="12270" tabRatio="822" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="11" r:id="rId1"/>
@@ -17,7 +17,8 @@
     <sheet name="Create_Group" sheetId="3" r:id="rId3"/>
     <sheet name="TermStore_Config" sheetId="4" r:id="rId4"/>
     <sheet name="Client_Config" sheetId="8" r:id="rId5"/>
-    <sheet name="Sample_Data" sheetId="9" r:id="rId6"/>
+    <sheet name="MatterAdditionalColumns" sheetId="12" r:id="rId6"/>
+    <sheet name="Sample_Data" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027" forceFullCalc="1"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="140">
   <si>
     <t>Group_Name</t>
   </si>
@@ -489,12 +490,81 @@
       <t>&lt;CATALOGNAME&gt;</t>
     </r>
   </si>
+  <si>
+    <t>SiteColumnName</t>
+  </si>
+  <si>
+    <t>ColumnType</t>
+  </si>
+  <si>
+    <t>SubColumnType</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>MatterAdditionalComments</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>_MatterCenter</t>
+  </si>
+  <si>
+    <t>IsClientCritical</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>MatterClosureDate</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>IsMatterDuplicate</t>
+  </si>
+  <si>
+    <t>MatterUploadOptions</t>
+  </si>
+  <si>
+    <t>Choice</t>
+  </si>
+  <si>
+    <t>RadioButtons</t>
+  </si>
+  <si>
+    <t>Emails, Attachments,Desktop</t>
+  </si>
+  <si>
+    <t>MatterRelatedTo</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>Patents,Copyrights,Infringements</t>
+  </si>
+  <si>
+    <t>MatterFiledAgainst</t>
+  </si>
+  <si>
+    <t>MultiChoice</t>
+  </si>
+  <si>
+    <t>Contoso,Fabrikam</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,8 +615,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -559,8 +647,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7D31"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -583,11 +677,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -626,6 +744,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -993,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1732,6 +1860,146 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O16"/>
   <sheetViews>

</xml_diff>